<commit_message>
Updated FMCG_stocks.xlsx with new data
</commit_message>
<xml_diff>
--- a/NAV/FMCG_stocks.xlsx
+++ b/NAV/FMCG_stocks.xlsx
@@ -460,7 +460,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J612"/>
+  <dimension ref="A1:J633"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A575" workbookViewId="0">
       <selection activeCell="G588" sqref="G588"/>
@@ -19475,6 +19475,657 @@
         <v>177.4530590978789</v>
       </c>
     </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>2024-08-28</t>
+        </is>
+      </c>
+      <c r="C613" t="n">
+        <v>661.9000244140625</v>
+      </c>
+      <c r="D613" t="n">
+        <v>1477.5</v>
+      </c>
+      <c r="E613" t="n">
+        <v>611.2000122070312</v>
+      </c>
+      <c r="F613" t="n">
+        <v>1308.050048828125</v>
+      </c>
+      <c r="G613" t="n">
+        <v>839.75</v>
+      </c>
+      <c r="H613" t="n">
+        <v>18182.55035400391</v>
+      </c>
+      <c r="I613" t="n">
+        <v>0</v>
+      </c>
+      <c r="J613" t="n">
+        <v>177.4530590978789</v>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>2024-08-29</t>
+        </is>
+      </c>
+      <c r="C614" t="n">
+        <v>660.75</v>
+      </c>
+      <c r="D614" t="n">
+        <v>1476.699951171875</v>
+      </c>
+      <c r="E614" t="n">
+        <v>603.6199951171875</v>
+      </c>
+      <c r="F614" t="n">
+        <v>1309.849975585938</v>
+      </c>
+      <c r="G614" t="n">
+        <v>813</v>
+      </c>
+      <c r="H614" t="n">
+        <v>18047.759765625</v>
+      </c>
+      <c r="I614" t="n">
+        <v>-0.007413183835854168</v>
+      </c>
+      <c r="J614" t="n">
+        <v>176.1375669485516</v>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>2024-08-30</t>
+        </is>
+      </c>
+      <c r="C615" t="n">
+        <v>647.1500244140625</v>
+      </c>
+      <c r="D615" t="n">
+        <v>1481.199951171875</v>
+      </c>
+      <c r="E615" t="n">
+        <v>600.3599853515625</v>
+      </c>
+      <c r="F615" t="n">
+        <v>1311.599975585938</v>
+      </c>
+      <c r="G615" t="n">
+        <v>813.2000122070312</v>
+      </c>
+      <c r="H615" t="n">
+        <v>17962.32995605469</v>
+      </c>
+      <c r="I615" t="n">
+        <v>-0.004733540931380745</v>
+      </c>
+      <c r="J615" t="n">
+        <v>175.3038125658468</v>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>2024-09-02</t>
+        </is>
+      </c>
+      <c r="C616" t="n">
+        <v>650.9500122070312</v>
+      </c>
+      <c r="D616" t="n">
+        <v>1470.050048828125</v>
+      </c>
+      <c r="E616" t="n">
+        <v>608.5800170898438</v>
+      </c>
+      <c r="F616" t="n">
+        <v>1316.800048828125</v>
+      </c>
+      <c r="G616" t="n">
+        <v>811.2000122070312</v>
+      </c>
+      <c r="H616" t="n">
+        <v>17987.74047851562</v>
+      </c>
+      <c r="I616" t="n">
+        <v>0.001414656256905703</v>
+      </c>
+      <c r="J616" t="n">
+        <v>175.5518072011525</v>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>2024-09-03</t>
+        </is>
+      </c>
+      <c r="C617" t="n">
+        <v>640.0499877929688</v>
+      </c>
+      <c r="D617" t="n">
+        <v>1460.75</v>
+      </c>
+      <c r="E617" t="n">
+        <v>599.9400024414062</v>
+      </c>
+      <c r="F617" t="n">
+        <v>1341.949951171875</v>
+      </c>
+      <c r="G617" t="n">
+        <v>822.3499755859375</v>
+      </c>
+      <c r="H617" t="n">
+        <v>17977.66967773438</v>
+      </c>
+      <c r="I617" t="n">
+        <v>-0.0005598702512568748</v>
+      </c>
+      <c r="J617" t="n">
+        <v>175.4535209667462</v>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>2024-09-04</t>
+        </is>
+      </c>
+      <c r="C618" t="n">
+        <v>645.5999755859375</v>
+      </c>
+      <c r="D618" t="n">
+        <v>1475.300048828125</v>
+      </c>
+      <c r="E618" t="n">
+        <v>609</v>
+      </c>
+      <c r="F618" t="n">
+        <v>1327.75</v>
+      </c>
+      <c r="G618" t="n">
+        <v>824.2999877929688</v>
+      </c>
+      <c r="H618" t="n">
+        <v>18052.54992675781</v>
+      </c>
+      <c r="I618" t="n">
+        <v>0.004165181047695957</v>
+      </c>
+      <c r="J618" t="n">
+        <v>176.1843166470284</v>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>2024-09-05</t>
+        </is>
+      </c>
+      <c r="C619" t="n">
+        <v>643.9000244140625</v>
+      </c>
+      <c r="D619" t="n">
+        <v>1457.699951171875</v>
+      </c>
+      <c r="E619" t="n">
+        <v>602.1799926757812</v>
+      </c>
+      <c r="F619" t="n">
+        <v>1254.800048828125</v>
+      </c>
+      <c r="G619" t="n">
+        <v>835.4000244140625</v>
+      </c>
+      <c r="H619" t="n">
+        <v>17792.94024658203</v>
+      </c>
+      <c r="I619" t="n">
+        <v>-0.01438077619112318</v>
+      </c>
+      <c r="J619" t="n">
+        <v>173.6506494209415</v>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>2024-09-06</t>
+        </is>
+      </c>
+      <c r="C620" t="n">
+        <v>665.25</v>
+      </c>
+      <c r="D620" t="n">
+        <v>1443.449951171875</v>
+      </c>
+      <c r="E620" t="n">
+        <v>597.2999877929688</v>
+      </c>
+      <c r="F620" t="n">
+        <v>1256.849975585938</v>
+      </c>
+      <c r="G620" t="n">
+        <v>832.7000122070312</v>
+      </c>
+      <c r="H620" t="n">
+        <v>17880.34979248047</v>
+      </c>
+      <c r="I620" t="n">
+        <v>0.004912597057432855</v>
+      </c>
+      <c r="J620" t="n">
+        <v>174.5037250903082</v>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>2024-09-09</t>
+        </is>
+      </c>
+      <c r="C621" t="n">
+        <v>676</v>
+      </c>
+      <c r="D621" t="n">
+        <v>1492.050048828125</v>
+      </c>
+      <c r="E621" t="n">
+        <v>610.3400268554688</v>
+      </c>
+      <c r="F621" t="n">
+        <v>1225.25</v>
+      </c>
+      <c r="G621" t="n">
+        <v>827.5999755859375</v>
+      </c>
+      <c r="H621" t="n">
+        <v>18025.32012939453</v>
+      </c>
+      <c r="I621" t="n">
+        <v>0.008107802061849448</v>
+      </c>
+      <c r="J621" t="n">
+        <v>175.9185667523958</v>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>2024-09-10</t>
+        </is>
+      </c>
+      <c r="C622" t="n">
+        <v>680</v>
+      </c>
+      <c r="D622" t="n">
+        <v>1503.050048828125</v>
+      </c>
+      <c r="E622" t="n">
+        <v>608</v>
+      </c>
+      <c r="F622" t="n">
+        <v>1246</v>
+      </c>
+      <c r="G622" t="n">
+        <v>824.75</v>
+      </c>
+      <c r="H622" t="n">
+        <v>18130.15014648438</v>
+      </c>
+      <c r="I622" t="n">
+        <v>0.005815709032478913</v>
+      </c>
+      <c r="J622" t="n">
+        <v>176.9416579500384</v>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>2024-09-11</t>
+        </is>
+      </c>
+      <c r="C623" t="n">
+        <v>680.4500122070312</v>
+      </c>
+      <c r="D623" t="n">
+        <v>1499.949951171875</v>
+      </c>
+      <c r="E623" t="n">
+        <v>627.6599731445312</v>
+      </c>
+      <c r="F623" t="n">
+        <v>1229</v>
+      </c>
+      <c r="G623" t="n">
+        <v>814</v>
+      </c>
+      <c r="H623" t="n">
+        <v>18088.97985839844</v>
+      </c>
+      <c r="I623" t="n">
+        <v>-0.002270818926114677</v>
+      </c>
+      <c r="J623" t="n">
+        <v>176.5398554843474</v>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>2024-09-12</t>
+        </is>
+      </c>
+      <c r="C624" t="n">
+        <v>686.0999755859375</v>
+      </c>
+      <c r="D624" t="n">
+        <v>1513.449951171875</v>
+      </c>
+      <c r="E624" t="n">
+        <v>645.5999755859375</v>
+      </c>
+      <c r="F624" t="n">
+        <v>1224.849975585938</v>
+      </c>
+      <c r="G624" t="n">
+        <v>809.7000122070312</v>
+      </c>
+      <c r="H624" t="n">
+        <v>18193.19958496094</v>
+      </c>
+      <c r="I624" t="n">
+        <v>0.00576150382046627</v>
+      </c>
+      <c r="J624" t="n">
+        <v>177.556990536185</v>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>2024-09-13</t>
+        </is>
+      </c>
+      <c r="C625" t="n">
+        <v>681.9500122070312</v>
+      </c>
+      <c r="D625" t="n">
+        <v>1491.300048828125</v>
+      </c>
+      <c r="E625" t="n">
+        <v>646.6500244140625</v>
+      </c>
+      <c r="F625" t="n">
+        <v>1229.300048828125</v>
+      </c>
+      <c r="G625" t="n">
+        <v>788.0499877929688</v>
+      </c>
+      <c r="H625" t="n">
+        <v>18027.60040283203</v>
+      </c>
+      <c r="I625" t="n">
+        <v>-0.009102257211853799</v>
+      </c>
+      <c r="J625" t="n">
+        <v>175.9408211385619</v>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>2024-09-16</t>
+        </is>
+      </c>
+      <c r="C626" t="n">
+        <v>695.2000122070312</v>
+      </c>
+      <c r="D626" t="n">
+        <v>1456.349975585938</v>
+      </c>
+      <c r="E626" t="n">
+        <v>621.0499877929688</v>
+      </c>
+      <c r="F626" t="n">
+        <v>1219.699951171875</v>
+      </c>
+      <c r="G626" t="n">
+        <v>751.9500122070312</v>
+      </c>
+      <c r="H626" t="n">
+        <v>17765.49987792969</v>
+      </c>
+      <c r="I626" t="n">
+        <v>-0.01453884704817227</v>
+      </c>
+      <c r="J626" t="n">
+        <v>173.3828444504985</v>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>2024-09-17</t>
+        </is>
+      </c>
+      <c r="C627" t="n">
+        <v>692</v>
+      </c>
+      <c r="D627" t="n">
+        <v>1459.400024414062</v>
+      </c>
+      <c r="E627" t="n">
+        <v>649.6500244140625</v>
+      </c>
+      <c r="F627" t="n">
+        <v>1222.949951171875</v>
+      </c>
+      <c r="G627" t="n">
+        <v>746.75</v>
+      </c>
+      <c r="H627" t="n">
+        <v>17827</v>
+      </c>
+      <c r="I627" t="n">
+        <v>0.003461772676980224</v>
+      </c>
+      <c r="J627" t="n">
+        <v>173.9830564440744</v>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>2024-09-18</t>
+        </is>
+      </c>
+      <c r="C628" t="n">
+        <v>695.2999877929688</v>
+      </c>
+      <c r="D628" t="n">
+        <v>1432.150024414062</v>
+      </c>
+      <c r="E628" t="n">
+        <v>646.7000122070312</v>
+      </c>
+      <c r="F628" t="n">
+        <v>1224.550048828125</v>
+      </c>
+      <c r="G628" t="n">
+        <v>744.5999755859375</v>
+      </c>
+      <c r="H628" t="n">
+        <v>17755.70007324219</v>
+      </c>
+      <c r="I628" t="n">
+        <v>-0.003999547133999692</v>
+      </c>
+      <c r="J628" t="n">
+        <v>173.287203009309</v>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>2024-09-19</t>
+        </is>
+      </c>
+      <c r="C629" t="n">
+        <v>697</v>
+      </c>
+      <c r="D629" t="n">
+        <v>1444.849975585938</v>
+      </c>
+      <c r="E629" t="n">
+        <v>652.1500244140625</v>
+      </c>
+      <c r="F629" t="n">
+        <v>1197.849975585938</v>
+      </c>
+      <c r="G629" t="n">
+        <v>747.2000122070312</v>
+      </c>
+      <c r="H629" t="n">
+        <v>17752.34997558594</v>
+      </c>
+      <c r="I629" t="n">
+        <v>-0.0001886773060161447</v>
+      </c>
+      <c r="J629" t="n">
+        <v>173.2545076466781</v>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>2024-09-20</t>
+        </is>
+      </c>
+      <c r="C630" t="n">
+        <v>709</v>
+      </c>
+      <c r="D630" t="n">
+        <v>1456.599975585938</v>
+      </c>
+      <c r="E630" t="n">
+        <v>654.4500122070312</v>
+      </c>
+      <c r="F630" t="n">
+        <v>1206.300048828125</v>
+      </c>
+      <c r="G630" t="n">
+        <v>747.5499877929688</v>
+      </c>
+      <c r="H630" t="n">
+        <v>17905.25006103516</v>
+      </c>
+      <c r="I630" t="n">
+        <v>0.008612949027001824</v>
+      </c>
+      <c r="J630" t="n">
+        <v>174.7467398897373</v>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>2024-09-23</t>
+        </is>
+      </c>
+      <c r="C631" t="n">
+        <v>702.5</v>
+      </c>
+      <c r="D631" t="n">
+        <v>1449.300048828125</v>
+      </c>
+      <c r="E631" t="n">
+        <v>654.0999755859375</v>
+      </c>
+      <c r="F631" t="n">
+        <v>1190</v>
+      </c>
+      <c r="G631" t="n">
+        <v>763.75</v>
+      </c>
+      <c r="H631" t="n">
+        <v>17852.70007324219</v>
+      </c>
+      <c r="I631" t="n">
+        <v>-0.00293489270542646</v>
+      </c>
+      <c r="J631" t="n">
+        <v>174.2338769575378</v>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>2024-09-24</t>
+        </is>
+      </c>
+      <c r="C632" t="n">
+        <v>705.0999755859375</v>
+      </c>
+      <c r="D632" t="n">
+        <v>1446.349975585938</v>
+      </c>
+      <c r="E632" t="n">
+        <v>646.8499755859375</v>
+      </c>
+      <c r="F632" t="n">
+        <v>1194.699951171875</v>
+      </c>
+      <c r="G632" t="n">
+        <v>760.9500122070312</v>
+      </c>
+      <c r="H632" t="n">
+        <v>17843.19958496094</v>
+      </c>
+      <c r="I632" t="n">
+        <v>-0.0005321597429113499</v>
+      </c>
+      <c r="J632" t="n">
+        <v>174.1411567023696</v>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>2024-09-25</t>
+        </is>
+      </c>
+      <c r="C633" t="n">
+        <v>689.2000122070312</v>
+      </c>
+      <c r="D633" t="n">
+        <v>1429.550048828125</v>
+      </c>
+      <c r="E633" t="n">
+        <v>633.2999877929688</v>
+      </c>
+      <c r="F633" t="n">
+        <v>1175.349975585938</v>
+      </c>
+      <c r="G633" t="n">
+        <v>742.5499877929688</v>
+      </c>
+      <c r="H633" t="n">
+        <v>17509.20007324219</v>
+      </c>
+      <c r="I633" t="n">
+        <v>-0.0187185885652627</v>
+      </c>
+      <c r="J633" t="n">
+        <v>170.8814800377791</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>